<commit_message>
Create async function to download published excel file
This function will download the file from server, and append data locally.
Over the next few commits constant names will be ironed out. Further,
implementation of saving and overwriting the file locally will occur.
That way, even if the server is down, the data can be loaded locally
onto the webpage.
</commit_message>
<xml_diff>
--- a/src/menu.xlsx
+++ b/src/menu.xlsx
@@ -1045,9 +1045,7 @@
       <c r="G37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="4"/>
@@ -1055,146 +1053,157 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39">
-      <c r="A39" s="1"/>
+    <row r="39" outlineLevel="1">
+      <c r="A39" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40">
+    <row r="40" outlineLevel="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="4"/>
       <c r="E40" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41">
+    <row r="41" outlineLevel="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="4"/>
       <c r="E41" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42">
+    <row r="42" outlineLevel="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="4"/>
       <c r="E42" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43">
+    <row r="43" outlineLevel="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="4"/>
       <c r="E43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44">
+    <row r="44" outlineLevel="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="4"/>
       <c r="E44" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45">
+    <row r="45" outlineLevel="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="4"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46">
+    <row r="46" outlineLevel="1">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47">
+    <row r="47" outlineLevel="1">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48">
+    <row r="48" outlineLevel="1">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49">
+    <row r="49" outlineLevel="1">
       <c r="A49" s="1"/>
       <c r="B49" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
+    </row>
+    <row r="50" outlineLevel="1">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>